<commit_message>
fixed eeprom in bom
</commit_message>
<xml_diff>
--- a/pcb/bom.xlsx
+++ b/pcb/bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20352"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20353"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwurzinger\Documents\GitHub\hardware\pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B97C34B8-CCB1-4063-8936-F03A8AD3C109}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7E6E9F-D9D9-4800-A2D6-83D9256C39C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bom" sheetId="1" r:id="rId1"/>
@@ -100,13 +100,13 @@
     <t>669-6058</t>
   </si>
   <si>
-    <t>800-9812</t>
+    <t>808-0199</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -951,11 +951,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1109,18 +1109,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display=" 674-2369"/>
-    <hyperlink ref="C3" r:id="rId2" display=" 681-2979"/>
-    <hyperlink ref="C4" r:id="rId3" display=" 681-2975"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="C7" r:id="rId6"/>
-    <hyperlink ref="C8" r:id="rId7" display=" 172-1482"/>
-    <hyperlink ref="C9" r:id="rId8"/>
-    <hyperlink ref="C10" r:id="rId9" display=" 135-9508"/>
-    <hyperlink ref="C11" r:id="rId10" display=" 540-2849"/>
-    <hyperlink ref="C12" r:id="rId11" display=" 669-6058"/>
-    <hyperlink ref="C13" r:id="rId12" display=" 800-9812"/>
+    <hyperlink ref="C2" r:id="rId1" display=" 674-2369" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" display=" 681-2979" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" display=" 681-2975" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C8" r:id="rId7" display=" 172-1482" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C10" r:id="rId9" display=" 135-9508" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C11" r:id="rId10" display=" 540-2849" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C12" r:id="rId11" display=" 669-6058" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>